<commit_message>
Agregar local con reponedor CENCOSUD
</commit_message>
<xml_diff>
--- a/Reponedores CENCOSUD.xlsx
+++ b/Reponedores CENCOSUD.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr showInkAnnotation="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Supermercados-Nacional\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC604F26-E700-47AE-AA78-0214C546B336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DA087DA-4332-4319-9FA2-F4942D4B51BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="747" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="757" uniqueCount="231">
   <si>
     <t>j775</t>
   </si>
@@ -719,6 +719,12 @@
   </si>
   <si>
     <t>SISA Pedro Fontova</t>
+  </si>
+  <si>
+    <t>Jumbo El Llano</t>
+  </si>
+  <si>
+    <t>J513</t>
   </si>
 </sst>
 </file>
@@ -930,8 +936,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFE2003-F3D9-42CC-9CBE-88474409C339}" name="Tabla1" displayName="Tabla1" ref="A1:G149" totalsRowShown="0">
-  <autoFilter ref="A1:G149" xr:uid="{7DFE2003-F3D9-42CC-9CBE-88474409C339}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{7DFE2003-F3D9-42CC-9CBE-88474409C339}" name="Tabla1" displayName="Tabla1" ref="A1:G151" totalsRowShown="0">
+  <autoFilter ref="A1:G151" xr:uid="{7DFE2003-F3D9-42CC-9CBE-88474409C339}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G75">
     <sortCondition ref="C1:C75"/>
   </sortState>
@@ -1245,10 +1251,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{714BCE76-32ED-E444-A031-ED290FE4EDA4}">
-  <dimension ref="A1:G149"/>
+  <dimension ref="A1:G151"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A122" zoomScale="91" zoomScaleNormal="91" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="G149" sqref="G149"/>
+    <sheetView tabSelected="1" topLeftCell="A133" zoomScale="91" zoomScaleNormal="91" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="A152" sqref="A152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4689,6 +4695,52 @@
         <v>6</v>
       </c>
     </row>
+    <row r="150" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A150" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="B150" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D150" s="37">
+        <v>4</v>
+      </c>
+      <c r="E150" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F150" s="36">
+        <v>5</v>
+      </c>
+      <c r="G150" s="36" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A151" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="B151" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="D151" s="37">
+        <v>4</v>
+      </c>
+      <c r="E151" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="F151" s="36">
+        <v>6</v>
+      </c>
+      <c r="G151" s="36" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>

</xml_diff>